<commit_message>
142‘’ git commit -m142‘
</commit_message>
<xml_diff>
--- a/Excel/AchievementConfig.xlsx
+++ b/Excel/AchievementConfig.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="192">
   <si>
     <t>#</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>支持23</t>
+  </si>
+  <si>
+    <t>套装-1</t>
   </si>
   <si>
     <t>支持24</t>
@@ -1642,8 +1645,8 @@
   <sheetPr/>
   <dimension ref="C2:K172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="I111" sqref="I111"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2303,31 +2306,34 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" s="5" customFormat="1" spans="3:10">
-      <c r="C25" s="5">
+    <row r="25" spans="3:11">
+      <c r="C25" s="6">
         <v>1020</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="5">
-        <v>1</v>
-      </c>
-      <c r="F25" s="5">
+      <c r="E25" s="6">
+        <v>1</v>
+      </c>
+      <c r="F25" s="6">
         <f t="shared" si="0"/>
         <v>480</v>
       </c>
-      <c r="G25" s="5">
-        <v>5</v>
-      </c>
-      <c r="H25" s="5">
-        <v>0</v>
-      </c>
-      <c r="I25" s="5">
-        <v>1</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>14</v>
+      <c r="G25" s="6">
+        <v>1</v>
+      </c>
+      <c r="H25" s="6">
+        <v>15</v>
+      </c>
+      <c r="I25" s="6">
+        <v>5</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="26" s="3" customFormat="1" spans="3:11">
@@ -2390,34 +2396,34 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="3:11">
-      <c r="C28" s="6">
+    <row r="28" s="5" customFormat="1" spans="3:11">
+      <c r="C28" s="5">
         <v>1023</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="6">
-        <v>1</v>
-      </c>
-      <c r="F28" s="6">
+      <c r="E28" s="5">
+        <v>1</v>
+      </c>
+      <c r="F28" s="5">
         <f t="shared" si="0"/>
         <v>552</v>
       </c>
-      <c r="G28" s="6">
-        <v>1</v>
-      </c>
-      <c r="H28" s="6">
-        <v>15</v>
-      </c>
-      <c r="I28" s="6">
-        <v>5</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>18</v>
+      <c r="G28" s="5">
+        <v>2</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="3:11">
@@ -2425,7 +2431,7 @@
         <v>1024</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E29" s="6">
         <v>1</v>
@@ -2455,7 +2461,7 @@
         <v>1025</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E30" s="6">
         <v>1</v>
@@ -2485,7 +2491,7 @@
         <v>1026</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E31" s="6">
         <v>1</v>
@@ -2510,31 +2516,34 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" s="2" customFormat="1" spans="3:10">
-      <c r="C32" s="2">
+    <row r="32" s="4" customFormat="1" spans="3:11">
+      <c r="C32" s="4">
         <v>1027</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E32" s="2">
-        <v>1</v>
-      </c>
-      <c r="F32" s="2">
+      <c r="D32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="4">
+        <v>1</v>
+      </c>
+      <c r="F32" s="4">
         <f t="shared" si="0"/>
         <v>648</v>
       </c>
-      <c r="G32" s="2">
-        <v>2</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
-      <c r="I32" s="2">
-        <v>1</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>14</v>
+      <c r="G32" s="4">
+        <v>1</v>
+      </c>
+      <c r="H32" s="4">
+        <v>15</v>
+      </c>
+      <c r="I32" s="4">
+        <v>5</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="3:11">
@@ -2542,7 +2551,7 @@
         <v>1028</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E33" s="6">
         <v>1</v>
@@ -2572,7 +2581,7 @@
         <v>1029</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E34" s="6">
         <v>1</v>
@@ -2602,7 +2611,7 @@
         <v>1030</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E35" s="3">
         <v>1</v>
@@ -2632,7 +2641,7 @@
         <v>1031</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E36" s="6">
         <v>1</v>
@@ -2662,7 +2671,7 @@
         <v>1032</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E37" s="6">
         <v>1</v>
@@ -2692,7 +2701,7 @@
         <v>1033</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E38" s="6">
         <v>1</v>
@@ -2722,7 +2731,7 @@
         <v>1034</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E39" s="6">
         <v>1</v>
@@ -2752,7 +2761,7 @@
         <v>1035</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E40" s="6">
         <v>1</v>
@@ -2782,7 +2791,7 @@
         <v>1036</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E41" s="6">
         <v>1</v>
@@ -2812,7 +2821,7 @@
         <v>1037</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E42" s="6">
         <v>1</v>
@@ -2842,7 +2851,7 @@
         <v>1038</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E43" s="6">
         <v>1</v>
@@ -2864,7 +2873,7 @@
         <v>14</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" s="3" customFormat="1" spans="3:11">
@@ -2872,7 +2881,7 @@
         <v>1039</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E44" s="3">
         <v>1</v>
@@ -2902,7 +2911,7 @@
         <v>1040</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E45" s="6">
         <v>1</v>
@@ -2932,7 +2941,7 @@
         <v>1041</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E46" s="6">
         <v>1</v>
@@ -2962,7 +2971,7 @@
         <v>1042</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E47" s="6">
         <v>1</v>
@@ -2992,7 +3001,7 @@
         <v>1043</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E48" s="6">
         <v>1</v>
@@ -3022,7 +3031,7 @@
         <v>1044</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E49" s="6">
         <v>1</v>
@@ -3052,7 +3061,7 @@
         <v>1045</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E50" s="6">
         <v>1</v>
@@ -3082,7 +3091,7 @@
         <v>1046</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E51" s="6">
         <v>1</v>
@@ -3112,7 +3121,7 @@
         <v>1047</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E52" s="6">
         <v>1</v>
@@ -3134,7 +3143,7 @@
         <v>14</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" s="3" customFormat="1" spans="3:11">
@@ -3142,7 +3151,7 @@
         <v>1048</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E53" s="3">
         <v>1</v>
@@ -3172,7 +3181,7 @@
         <v>1049</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E54" s="6">
         <v>1</v>
@@ -3197,34 +3206,31 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="3:11">
+    <row r="55" s="2" customFormat="1" spans="3:10">
       <c r="C55" s="6">
         <v>1050</v>
       </c>
-      <c r="D55" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E55" s="6">
-        <v>1</v>
-      </c>
-      <c r="F55" s="6">
+      <c r="D55" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="G55" s="6">
-        <v>1</v>
-      </c>
-      <c r="H55" s="6">
-        <v>15</v>
-      </c>
-      <c r="I55" s="6">
-        <v>5</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K55" s="6" t="s">
-        <v>18</v>
+      <c r="G55" s="2">
+        <v>5</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0</v>
+      </c>
+      <c r="I55" s="2">
+        <v>1</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="3:11">
@@ -3232,7 +3238,7 @@
         <v>1051</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E56" s="6">
         <v>1</v>
@@ -3262,7 +3268,7 @@
         <v>1052</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E57" s="6">
         <v>1</v>
@@ -3292,7 +3298,7 @@
         <v>1053</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E58" s="6">
         <v>1</v>
@@ -3322,7 +3328,7 @@
         <v>1054</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E59" s="6">
         <v>1</v>
@@ -3352,7 +3358,7 @@
         <v>1055</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E60" s="6">
         <v>1</v>
@@ -3382,7 +3388,7 @@
         <v>1056</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E61" s="6">
         <v>1</v>
@@ -3404,7 +3410,7 @@
         <v>14</v>
       </c>
       <c r="K61" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" s="3" customFormat="1" spans="3:11">
@@ -3412,7 +3418,7 @@
         <v>1057</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E62" s="3">
         <v>1</v>
@@ -3442,7 +3448,7 @@
         <v>1058</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E63" s="6">
         <v>1</v>
@@ -3472,7 +3478,7 @@
         <v>1059</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E64" s="6">
         <v>1</v>
@@ -3502,7 +3508,7 @@
         <v>1060</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E65" s="6">
         <v>1</v>
@@ -3532,7 +3538,7 @@
         <v>1061</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E66" s="6">
         <v>1</v>
@@ -3562,7 +3568,7 @@
         <v>1062</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E67" s="6">
         <v>1</v>
@@ -3592,7 +3598,7 @@
         <v>1063</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E68" s="6">
         <v>1</v>
@@ -3622,7 +3628,7 @@
         <v>1064</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E69" s="6">
         <v>1</v>
@@ -3652,7 +3658,7 @@
         <v>1065</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E70" s="6">
         <v>1</v>
@@ -3674,7 +3680,7 @@
         <v>14</v>
       </c>
       <c r="K70" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" s="3" customFormat="1" spans="3:11">
@@ -3682,7 +3688,7 @@
         <v>1066</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E71" s="3">
         <v>1</v>
@@ -3712,7 +3718,7 @@
         <v>2001</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E77" s="6">
         <v>2</v>
@@ -3731,7 +3737,7 @@
         <v>3</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K77" s="6" t="s">
         <v>15</v>
@@ -3742,7 +3748,7 @@
         <v>2002</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E78" s="6">
         <v>2</v>
@@ -3761,7 +3767,7 @@
         <v>3</v>
       </c>
       <c r="J78" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K78" s="6" t="s">
         <v>18</v>
@@ -3772,7 +3778,7 @@
         <v>2003</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E79" s="6">
         <v>2</v>
@@ -3791,7 +3797,7 @@
         <v>3</v>
       </c>
       <c r="J79" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K79" s="6" t="s">
         <v>20</v>
@@ -3802,7 +3808,7 @@
         <v>2004</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E80" s="6">
         <v>2</v>
@@ -3821,10 +3827,10 @@
         <v>3</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="3:11">
@@ -3832,7 +3838,7 @@
         <v>2005</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E81" s="6">
         <v>2</v>
@@ -3851,10 +3857,10 @@
         <v>3</v>
       </c>
       <c r="J81" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K81" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" spans="3:11">
@@ -3862,7 +3868,7 @@
         <v>2006</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E82" s="6">
         <v>2</v>
@@ -3881,10 +3887,10 @@
         <v>3</v>
       </c>
       <c r="J82" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K82" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="3:11">
@@ -3892,7 +3898,7 @@
         <v>2007</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E83" s="6">
         <v>2</v>
@@ -3911,10 +3917,10 @@
         <v>3</v>
       </c>
       <c r="J83" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="3:11">
@@ -3922,7 +3928,7 @@
         <v>2008</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E84" s="6">
         <v>2</v>
@@ -3941,10 +3947,10 @@
         <v>5</v>
       </c>
       <c r="J84" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K84" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="85" spans="3:11">
@@ -3952,7 +3958,7 @@
         <v>2009</v>
       </c>
       <c r="D85" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E85" s="6">
         <v>2</v>
@@ -3971,10 +3977,10 @@
         <v>5</v>
       </c>
       <c r="J85" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="86" s="3" customFormat="1" spans="3:11">
@@ -3982,7 +3988,7 @@
         <v>2010</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E86" s="3">
         <v>2</v>
@@ -4001,10 +4007,10 @@
         <v>5</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K86" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="3:11">
@@ -4012,7 +4018,7 @@
         <v>2011</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E87" s="6">
         <v>2</v>
@@ -4031,7 +4037,7 @@
         <v>3</v>
       </c>
       <c r="J87" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K87" s="6" t="s">
         <v>15</v>
@@ -4042,7 +4048,7 @@
         <v>2012</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E88" s="6">
         <v>2</v>
@@ -4061,7 +4067,7 @@
         <v>3</v>
       </c>
       <c r="J88" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K88" s="6" t="s">
         <v>18</v>
@@ -4072,7 +4078,7 @@
         <v>2013</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E89" s="6">
         <v>2</v>
@@ -4091,7 +4097,7 @@
         <v>3</v>
       </c>
       <c r="J89" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K89" s="6" t="s">
         <v>20</v>
@@ -4102,7 +4108,7 @@
         <v>2014</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E90" s="6">
         <v>2</v>
@@ -4121,10 +4127,10 @@
         <v>3</v>
       </c>
       <c r="J90" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="91" spans="3:11">
@@ -4132,7 +4138,7 @@
         <v>2015</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E91" s="6">
         <v>2</v>
@@ -4151,10 +4157,10 @@
         <v>3</v>
       </c>
       <c r="J91" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="92" spans="3:11">
@@ -4162,7 +4168,7 @@
         <v>2016</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E92" s="6">
         <v>2</v>
@@ -4181,10 +4187,10 @@
         <v>3</v>
       </c>
       <c r="J92" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K92" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="93" spans="3:11">
@@ -4192,7 +4198,7 @@
         <v>2017</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E93" s="6">
         <v>2</v>
@@ -4211,10 +4217,10 @@
         <v>3</v>
       </c>
       <c r="J93" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K93" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="94" spans="3:11">
@@ -4222,7 +4228,7 @@
         <v>2018</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E94" s="6">
         <v>2</v>
@@ -4241,10 +4247,10 @@
         <v>5</v>
       </c>
       <c r="J94" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K94" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="95" spans="3:11">
@@ -4252,7 +4258,7 @@
         <v>2019</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E95" s="6">
         <v>2</v>
@@ -4271,10 +4277,10 @@
         <v>5</v>
       </c>
       <c r="J95" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K95" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" s="3" customFormat="1" spans="3:11">
@@ -4282,7 +4288,7 @@
         <v>2020</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E96" s="3">
         <v>2</v>
@@ -4301,10 +4307,10 @@
         <v>5</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K96" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="3:11">
@@ -4312,7 +4318,7 @@
         <v>2021</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E97" s="6">
         <v>2</v>
@@ -4331,7 +4337,7 @@
         <v>3</v>
       </c>
       <c r="J97" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K97" s="6" t="s">
         <v>15</v>
@@ -4342,7 +4348,7 @@
         <v>2022</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E98" s="6">
         <v>2</v>
@@ -4361,7 +4367,7 @@
         <v>3</v>
       </c>
       <c r="J98" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K98" s="6" t="s">
         <v>18</v>
@@ -4372,7 +4378,7 @@
         <v>2023</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E99" s="6">
         <v>2</v>
@@ -4391,7 +4397,7 @@
         <v>3</v>
       </c>
       <c r="J99" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K99" s="6" t="s">
         <v>20</v>
@@ -4402,7 +4408,7 @@
         <v>2024</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E100" s="6">
         <v>2</v>
@@ -4421,10 +4427,10 @@
         <v>3</v>
       </c>
       <c r="J100" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K100" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="3:11">
@@ -4432,7 +4438,7 @@
         <v>2025</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E101" s="6">
         <v>2</v>
@@ -4451,10 +4457,10 @@
         <v>3</v>
       </c>
       <c r="J101" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K101" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="102" spans="3:11">
@@ -4462,7 +4468,7 @@
         <v>2026</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E102" s="6">
         <v>2</v>
@@ -4481,10 +4487,10 @@
         <v>3</v>
       </c>
       <c r="J102" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K102" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="103" spans="3:11">
@@ -4492,7 +4498,7 @@
         <v>2027</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E103" s="6">
         <v>2</v>
@@ -4511,10 +4517,10 @@
         <v>3</v>
       </c>
       <c r="J103" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K103" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="3:11">
@@ -4522,7 +4528,7 @@
         <v>2028</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E104" s="6">
         <v>2</v>
@@ -4541,10 +4547,10 @@
         <v>5</v>
       </c>
       <c r="J104" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K104" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="3:11">
@@ -4552,7 +4558,7 @@
         <v>2029</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E105" s="6">
         <v>2</v>
@@ -4571,10 +4577,10 @@
         <v>5</v>
       </c>
       <c r="J105" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K105" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="106" s="3" customFormat="1" spans="3:11">
@@ -4582,7 +4588,7 @@
         <v>2030</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E106" s="3">
         <v>2</v>
@@ -4601,10 +4607,10 @@
         <v>5</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K106" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="107" spans="3:11">
@@ -4612,7 +4618,7 @@
         <v>2031</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E107" s="6">
         <v>2</v>
@@ -4631,7 +4637,7 @@
         <v>3</v>
       </c>
       <c r="J107" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K107" s="6" t="s">
         <v>15</v>
@@ -4642,7 +4648,7 @@
         <v>2032</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E108" s="6">
         <v>2</v>
@@ -4661,7 +4667,7 @@
         <v>3</v>
       </c>
       <c r="J108" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K108" s="6" t="s">
         <v>18</v>
@@ -4672,7 +4678,7 @@
         <v>2033</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E109" s="6">
         <v>2</v>
@@ -4691,7 +4697,7 @@
         <v>3</v>
       </c>
       <c r="J109" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K109" s="6" t="s">
         <v>20</v>
@@ -4702,7 +4708,7 @@
         <v>2034</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E110" s="6">
         <v>2</v>
@@ -4721,10 +4727,10 @@
         <v>3</v>
       </c>
       <c r="J110" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K110" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="3:11">
@@ -4732,7 +4738,7 @@
         <v>2035</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E111" s="6">
         <v>2</v>
@@ -4751,10 +4757,10 @@
         <v>3</v>
       </c>
       <c r="J111" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K111" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="112" spans="3:11">
@@ -4762,7 +4768,7 @@
         <v>2036</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E112" s="6">
         <v>2</v>
@@ -4781,10 +4787,10 @@
         <v>3</v>
       </c>
       <c r="J112" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K112" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="113" spans="3:11">
@@ -4792,7 +4798,7 @@
         <v>2037</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E113" s="6">
         <v>2</v>
@@ -4811,10 +4817,10 @@
         <v>3</v>
       </c>
       <c r="J113" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K113" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="114" spans="3:11">
@@ -4822,7 +4828,7 @@
         <v>2038</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E114" s="6">
         <v>2</v>
@@ -4841,10 +4847,10 @@
         <v>5</v>
       </c>
       <c r="J114" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K114" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="115" spans="3:11">
@@ -4852,7 +4858,7 @@
         <v>2039</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E115" s="6">
         <v>2</v>
@@ -4871,10 +4877,10 @@
         <v>5</v>
       </c>
       <c r="J115" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K115" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="116" s="3" customFormat="1" spans="3:11">
@@ -4882,7 +4888,7 @@
         <v>2040</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E116" s="3">
         <v>2</v>
@@ -4901,10 +4907,10 @@
         <v>5</v>
       </c>
       <c r="J116" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K116" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="119" spans="3:10">
@@ -4912,7 +4918,7 @@
         <v>3001</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E119" s="6">
         <v>3</v>
@@ -4930,7 +4936,7 @@
         <v>5</v>
       </c>
       <c r="J119" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="3:10">
@@ -4938,7 +4944,7 @@
         <v>3002</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E120" s="6">
         <v>3</v>
@@ -4956,7 +4962,7 @@
         <v>5</v>
       </c>
       <c r="J120" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="121" spans="3:10">
@@ -4964,7 +4970,7 @@
         <v>3003</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E121" s="6">
         <v>3</v>
@@ -4982,7 +4988,7 @@
         <v>5</v>
       </c>
       <c r="J121" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="122" spans="3:10">
@@ -4990,7 +4996,7 @@
         <v>3004</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E122" s="6">
         <v>3</v>
@@ -5008,7 +5014,7 @@
         <v>5</v>
       </c>
       <c r="J122" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="123" spans="3:10">
@@ -5016,7 +5022,7 @@
         <v>3005</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E123" s="6">
         <v>3</v>
@@ -5034,7 +5040,7 @@
         <v>5</v>
       </c>
       <c r="J123" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="124" spans="3:10">
@@ -5042,7 +5048,7 @@
         <v>3006</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E124" s="6">
         <v>3</v>
@@ -5060,7 +5066,7 @@
         <v>5</v>
       </c>
       <c r="J124" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125" spans="3:10">
@@ -5068,7 +5074,7 @@
         <v>3007</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E125" s="6">
         <v>3</v>
@@ -5086,7 +5092,7 @@
         <v>5</v>
       </c>
       <c r="J125" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="126" spans="3:10">
@@ -5094,7 +5100,7 @@
         <v>3008</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E126" s="6">
         <v>3</v>
@@ -5112,7 +5118,7 @@
         <v>5</v>
       </c>
       <c r="J126" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="127" spans="3:10">
@@ -5120,7 +5126,7 @@
         <v>3009</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E127" s="6">
         <v>3</v>
@@ -5138,7 +5144,7 @@
         <v>5</v>
       </c>
       <c r="J127" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="128" spans="3:10">
@@ -5146,7 +5152,7 @@
         <v>3010</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E128" s="6">
         <v>3</v>
@@ -5164,7 +5170,7 @@
         <v>5</v>
       </c>
       <c r="J128" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="131" spans="3:10">
@@ -5172,7 +5178,7 @@
         <v>4001</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E131" s="6">
         <v>4</v>
@@ -5190,7 +5196,7 @@
         <v>1</v>
       </c>
       <c r="J131" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="132" spans="3:10">
@@ -5198,7 +5204,7 @@
         <v>4002</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E132" s="6">
         <v>4</v>
@@ -5216,7 +5222,7 @@
         <v>1</v>
       </c>
       <c r="J132" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="133" spans="3:10">
@@ -5224,7 +5230,7 @@
         <v>4003</v>
       </c>
       <c r="D133" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E133" s="6">
         <v>4</v>
@@ -5242,7 +5248,7 @@
         <v>1</v>
       </c>
       <c r="J133" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="134" spans="3:10">
@@ -5250,7 +5256,7 @@
         <v>4004</v>
       </c>
       <c r="D134" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E134" s="6">
         <v>4</v>
@@ -5268,7 +5274,7 @@
         <v>1</v>
       </c>
       <c r="J134" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="135" spans="3:10">
@@ -5276,7 +5282,7 @@
         <v>4005</v>
       </c>
       <c r="D135" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E135" s="6">
         <v>4</v>
@@ -5294,7 +5300,7 @@
         <v>1</v>
       </c>
       <c r="J135" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="136" spans="3:10">
@@ -5302,7 +5308,7 @@
         <v>4006</v>
       </c>
       <c r="D136" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E136" s="6">
         <v>4</v>
@@ -5320,7 +5326,7 @@
         <v>1</v>
       </c>
       <c r="J136" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="137" spans="3:10">
@@ -5328,7 +5334,7 @@
         <v>4007</v>
       </c>
       <c r="D137" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E137" s="6">
         <v>4</v>
@@ -5346,7 +5352,7 @@
         <v>1</v>
       </c>
       <c r="J137" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="138" spans="3:10">
@@ -5354,7 +5360,7 @@
         <v>4008</v>
       </c>
       <c r="D138" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E138" s="6">
         <v>4</v>
@@ -5372,7 +5378,7 @@
         <v>1</v>
       </c>
       <c r="J138" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="139" spans="3:10">
@@ -5380,7 +5386,7 @@
         <v>4009</v>
       </c>
       <c r="D139" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E139" s="6">
         <v>4</v>
@@ -5398,7 +5404,7 @@
         <v>1</v>
       </c>
       <c r="J139" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="140" spans="3:10">
@@ -5406,7 +5412,7 @@
         <v>4010</v>
       </c>
       <c r="D140" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E140" s="6">
         <v>4</v>
@@ -5424,7 +5430,7 @@
         <v>1</v>
       </c>
       <c r="J140" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="142" spans="3:10">
@@ -5432,7 +5438,7 @@
         <v>5001</v>
       </c>
       <c r="D142" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E142" s="6">
         <v>5</v>
@@ -5451,7 +5457,7 @@
         <v>5</v>
       </c>
       <c r="J142" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="143" spans="3:10">
@@ -5459,7 +5465,7 @@
         <v>5002</v>
       </c>
       <c r="D143" s="6" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E143" s="6">
         <v>5</v>
@@ -5478,7 +5484,7 @@
         <v>5</v>
       </c>
       <c r="J143" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="144" spans="3:10">
@@ -5486,7 +5492,7 @@
         <v>5003</v>
       </c>
       <c r="D144" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E144" s="6">
         <v>5</v>
@@ -5505,7 +5511,7 @@
         <v>5</v>
       </c>
       <c r="J144" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="145" spans="3:10">
@@ -5513,7 +5519,7 @@
         <v>5004</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E145" s="6">
         <v>5</v>
@@ -5532,7 +5538,7 @@
         <v>5</v>
       </c>
       <c r="J145" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="146" spans="3:10">
@@ -5540,7 +5546,7 @@
         <v>5005</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E146" s="6">
         <v>5</v>
@@ -5559,7 +5565,7 @@
         <v>5</v>
       </c>
       <c r="J146" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="147" spans="3:10">
@@ -5567,7 +5573,7 @@
         <v>5006</v>
       </c>
       <c r="D147" s="6" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E147" s="6">
         <v>5</v>
@@ -5586,7 +5592,7 @@
         <v>5</v>
       </c>
       <c r="J147" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="3:10">
@@ -5594,7 +5600,7 @@
         <v>5007</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E148" s="6">
         <v>5</v>
@@ -5613,7 +5619,7 @@
         <v>5</v>
       </c>
       <c r="J148" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="149" spans="3:10">
@@ -5621,7 +5627,7 @@
         <v>5008</v>
       </c>
       <c r="D149" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E149" s="6">
         <v>5</v>
@@ -5640,7 +5646,7 @@
         <v>5</v>
       </c>
       <c r="J149" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="150" spans="3:10">
@@ -5648,7 +5654,7 @@
         <v>5009</v>
       </c>
       <c r="D150" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E150" s="6">
         <v>5</v>
@@ -5667,7 +5673,7 @@
         <v>5</v>
       </c>
       <c r="J150" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="151" spans="3:10">
@@ -5675,7 +5681,7 @@
         <v>5010</v>
       </c>
       <c r="D151" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E151" s="6">
         <v>5</v>
@@ -5694,7 +5700,7 @@
         <v>5</v>
       </c>
       <c r="J151" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="152" spans="3:10">
@@ -5702,7 +5708,7 @@
         <v>5011</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E152" s="6">
         <v>5</v>
@@ -5721,7 +5727,7 @@
         <v>5</v>
       </c>
       <c r="J152" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="153" spans="3:10">
@@ -5729,7 +5735,7 @@
         <v>5012</v>
       </c>
       <c r="D153" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E153" s="6">
         <v>5</v>
@@ -5748,7 +5754,7 @@
         <v>5</v>
       </c>
       <c r="J153" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="154" spans="3:10">
@@ -5756,7 +5762,7 @@
         <v>5013</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E154" s="6">
         <v>5</v>
@@ -5775,7 +5781,7 @@
         <v>5</v>
       </c>
       <c r="J154" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="155" spans="3:10">
@@ -5783,7 +5789,7 @@
         <v>5014</v>
       </c>
       <c r="D155" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E155" s="6">
         <v>5</v>
@@ -5802,7 +5808,7 @@
         <v>5</v>
       </c>
       <c r="J155" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="156" spans="3:10">
@@ -5810,7 +5816,7 @@
         <v>5015</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E156" s="6">
         <v>5</v>
@@ -5829,7 +5835,7 @@
         <v>5</v>
       </c>
       <c r="J156" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="157" spans="3:10">
@@ -5837,7 +5843,7 @@
         <v>5016</v>
       </c>
       <c r="D157" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E157" s="6">
         <v>5</v>
@@ -5856,7 +5862,7 @@
         <v>5</v>
       </c>
       <c r="J157" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="158" spans="3:10">
@@ -5864,7 +5870,7 @@
         <v>5017</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E158" s="6">
         <v>5</v>
@@ -5883,7 +5889,7 @@
         <v>5</v>
       </c>
       <c r="J158" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="159" spans="3:10">
@@ -5891,7 +5897,7 @@
         <v>5018</v>
       </c>
       <c r="D159" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E159" s="6">
         <v>5</v>
@@ -5910,7 +5916,7 @@
         <v>5</v>
       </c>
       <c r="J159" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="160" spans="3:10">
@@ -5918,7 +5924,7 @@
         <v>5019</v>
       </c>
       <c r="D160" s="6" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E160" s="6">
         <v>5</v>
@@ -5937,7 +5943,7 @@
         <v>5</v>
       </c>
       <c r="J160" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="161" spans="3:10">
@@ -5945,7 +5951,7 @@
         <v>5020</v>
       </c>
       <c r="D161" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E161" s="6">
         <v>5</v>
@@ -5964,7 +5970,7 @@
         <v>5</v>
       </c>
       <c r="J161" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="163" spans="3:10">
@@ -5972,7 +5978,7 @@
         <v>6001</v>
       </c>
       <c r="D163" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E163" s="6">
         <v>6</v>
@@ -5990,7 +5996,7 @@
         <v>1</v>
       </c>
       <c r="J163" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="164" spans="3:10">
@@ -5998,7 +6004,7 @@
         <v>6002</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E164" s="6">
         <v>6</v>
@@ -6016,7 +6022,7 @@
         <v>1</v>
       </c>
       <c r="J164" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="165" spans="3:10">
@@ -6024,7 +6030,7 @@
         <v>6003</v>
       </c>
       <c r="D165" s="6" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E165" s="6">
         <v>6</v>
@@ -6042,7 +6048,7 @@
         <v>1</v>
       </c>
       <c r="J165" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="166" spans="3:10">
@@ -6050,7 +6056,7 @@
         <v>6004</v>
       </c>
       <c r="D166" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E166" s="6">
         <v>6</v>
@@ -6068,7 +6074,7 @@
         <v>1</v>
       </c>
       <c r="J166" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="167" spans="3:10">
@@ -6076,7 +6082,7 @@
         <v>6005</v>
       </c>
       <c r="D167" s="6" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E167" s="6">
         <v>6</v>
@@ -6094,7 +6100,7 @@
         <v>1</v>
       </c>
       <c r="J167" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="168" spans="3:10">
@@ -6102,7 +6108,7 @@
         <v>6006</v>
       </c>
       <c r="D168" s="6" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E168" s="6">
         <v>6</v>
@@ -6120,7 +6126,7 @@
         <v>1</v>
       </c>
       <c r="J168" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="169" spans="3:10">
@@ -6128,7 +6134,7 @@
         <v>6007</v>
       </c>
       <c r="D169" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E169" s="6">
         <v>6</v>
@@ -6146,7 +6152,7 @@
         <v>1</v>
       </c>
       <c r="J169" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="170" spans="3:10">
@@ -6154,7 +6160,7 @@
         <v>6008</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E170" s="6">
         <v>6</v>
@@ -6172,7 +6178,7 @@
         <v>1</v>
       </c>
       <c r="J170" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="171" spans="3:10">
@@ -6180,7 +6186,7 @@
         <v>6009</v>
       </c>
       <c r="D171" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E171" s="6">
         <v>6</v>
@@ -6198,7 +6204,7 @@
         <v>1</v>
       </c>
       <c r="J171" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="172" spans="3:10">
@@ -6206,7 +6212,7 @@
         <v>6010</v>
       </c>
       <c r="D172" s="6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E172" s="6">
         <v>6</v>
@@ -6224,7 +6230,7 @@
         <v>1</v>
       </c>
       <c r="J172" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>